<commit_message>
Fixed example input s/sheets
</commit_message>
<xml_diff>
--- a/example-input/v4_E-MTAB-5061-small.xlsx
+++ b/example-input/v4_E-MTAB-5061-small.xlsx
@@ -14,9 +14,9 @@
     <sheet name="contact.contributors" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="sample.donor" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="sample.specimen_from_organism" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="sample.specimen_from_organism.state_of_specimen" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="state_of_specimen" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="sample.cell_suspension" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="sample.cell_suspension.enrichment" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="cell_suspension.enrichment" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="sample.cell_suspension.well" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="single_cell" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="single_cell.barcode" sheetId="12" state="visible" r:id="rId13"/>
@@ -2991,7 +2991,7 @@
   <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3517,7 +3517,7 @@
   <dimension ref="A1:AC101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7983,7 +7983,7 @@
   <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8322,7 +8322,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8863,8 +8863,8 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC10" activeCellId="0" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9490,8 +9490,8 @@
   </sheetPr>
   <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14586,7 +14586,7 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>